<commit_message>
Q2 second revision data update
</commit_message>
<xml_diff>
--- a/data/haver_pivoted.xlsx
+++ b/data/haver_pivoted.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
@@ -875,7 +875,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
   <fonts count="1">
     <font>
@@ -1194,10 +1194,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
@@ -2444,7 +2444,7 @@
         <v>22038.2</v>
       </c>
       <c r="GY2" t="n">
-        <v>22722.6</v>
+        <v>22731.4</v>
       </c>
     </row>
     <row r="3">
@@ -3067,7 +3067,7 @@
         <v>19055.7</v>
       </c>
       <c r="GY3" t="n">
-        <v>19358.2</v>
+        <v>19360.6</v>
       </c>
     </row>
     <row r="4">
@@ -3690,7 +3690,7 @@
         <v>115.826</v>
       </c>
       <c r="GY4" t="n">
-        <v>117.519</v>
+        <v>117.547</v>
       </c>
     </row>
     <row r="5">
@@ -4313,7 +4313,7 @@
         <v>15005.4</v>
       </c>
       <c r="GY5" t="n">
-        <v>15672.6</v>
+        <v>15675.9</v>
       </c>
     </row>
     <row r="6">
@@ -4936,7 +4936,7 @@
         <v>13282.7</v>
       </c>
       <c r="GY6" t="n">
-        <v>13659.3</v>
+        <v>13660.2</v>
       </c>
     </row>
     <row r="7">
@@ -5559,7 +5559,7 @@
         <v>112.989</v>
       </c>
       <c r="GY7" t="n">
-        <v>114.758</v>
+        <v>114.775</v>
       </c>
     </row>
     <row r="8">
@@ -6182,7 +6182,7 @@
         <v>114.065</v>
       </c>
       <c r="GY8" t="n">
-        <v>115.176</v>
+        <v>115.19</v>
       </c>
     </row>
     <row r="9">
@@ -6805,7 +6805,7 @@
         <v>119.416</v>
       </c>
       <c r="GY9" t="n">
-        <v>121.48</v>
+        <v>121.509</v>
       </c>
     </row>
     <row r="10">
@@ -7428,7 +7428,7 @@
         <v>119.419</v>
       </c>
       <c r="GY10" t="n">
-        <v>121.38</v>
+        <v>121.397</v>
       </c>
     </row>
     <row r="11">
@@ -8051,7 +8051,7 @@
         <v>119.416</v>
       </c>
       <c r="GY11" t="n">
-        <v>121.95</v>
+        <v>122.035</v>
       </c>
     </row>
     <row r="12">
@@ -9297,7 +9297,7 @@
         <v>695.9</v>
       </c>
       <c r="GY13" t="n">
-        <v>712.9</v>
+        <v>735.5</v>
       </c>
     </row>
     <row r="14">
@@ -9920,7 +9920,7 @@
         <v>565.8</v>
       </c>
       <c r="GY14" t="n">
-        <v>482.1</v>
+        <v>480.5</v>
       </c>
     </row>
     <row r="15">
@@ -10543,7 +10543,7 @@
         <v>5920.6</v>
       </c>
       <c r="GY15" t="n">
-        <v>4237.1</v>
+        <v>4257.9</v>
       </c>
     </row>
     <row r="16">
@@ -11166,7 +11166,7 @@
         <v>115.3</v>
       </c>
       <c r="GY16" t="n">
-        <v>115.8</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17">
@@ -11786,10 +11786,10 @@
         <v>2259.8</v>
       </c>
       <c r="GX17" t="n">
-        <v>2318.7</v>
+        <v>2412.1</v>
       </c>
       <c r="GY17" t="n">
-        <v>2427.5</v>
+        <v>2550.4</v>
       </c>
     </row>
     <row r="18">
@@ -12412,7 +12412,7 @@
         <v>1580.1</v>
       </c>
       <c r="GY18" t="n">
-        <v>1640.6</v>
+        <v>1640.2</v>
       </c>
     </row>
     <row r="19">
@@ -13035,7 +13035,7 @@
         <v>331.9</v>
       </c>
       <c r="GY19" t="n">
-        <v>308.133333333333</v>
+        <v>351.7</v>
       </c>
     </row>
     <row r="20">
@@ -13658,7 +13658,7 @@
         <v>3977.3</v>
       </c>
       <c r="GY20" t="n">
-        <v>4018.9</v>
+        <v>4016</v>
       </c>
     </row>
     <row r="21">
@@ -14281,7 +14281,7 @@
         <v>1539.2</v>
       </c>
       <c r="GY21" t="n">
-        <v>1562.7</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="22">
@@ -14904,7 +14904,7 @@
         <v>112.97</v>
       </c>
       <c r="GY22" t="n">
-        <v>114.739</v>
+        <v>114.756</v>
       </c>
     </row>
     <row r="23">
@@ -15527,7 +15527,7 @@
         <v>1568.6</v>
       </c>
       <c r="GY23" t="n">
-        <v>1563.6</v>
+        <v>1563.3</v>
       </c>
     </row>
     <row r="24">
@@ -16150,7 +16150,7 @@
         <v>2408.7</v>
       </c>
       <c r="GY24" t="n">
-        <v>2455.4</v>
+        <v>2452.7</v>
       </c>
     </row>
     <row r="25">
@@ -16773,7 +16773,7 @@
         <v>1375.2</v>
       </c>
       <c r="GY25" t="n">
-        <v>1357.6</v>
+        <v>1357.1</v>
       </c>
     </row>
     <row r="26">
@@ -17396,7 +17396,7 @@
         <v>2017.1</v>
       </c>
       <c r="GY26" t="n">
-        <v>2021.2</v>
+        <v>2018.5</v>
       </c>
     </row>
     <row r="27">
@@ -18016,10 +18016,10 @@
         <v>1736.9</v>
       </c>
       <c r="GX27" t="n">
-        <v>1758.6</v>
+        <v>1851.9</v>
       </c>
       <c r="GY27" t="n">
-        <v>1808.6</v>
+        <v>1927.2</v>
       </c>
     </row>
     <row r="28">
@@ -18642,7 +18642,7 @@
         <v>166.2</v>
       </c>
       <c r="GY28" t="n">
-        <v>177.2</v>
+        <v>177.6</v>
       </c>
     </row>
     <row r="29">
@@ -19265,7 +19265,7 @@
         <v>246.4</v>
       </c>
       <c r="GY29" t="n">
-        <v>227.733333333333</v>
+        <v>261.2</v>
       </c>
     </row>
     <row r="30">
@@ -19888,7 +19888,7 @@
         <v>1517.9</v>
       </c>
       <c r="GY30" t="n">
-        <v>1540.8</v>
+        <v>1542.1</v>
       </c>
     </row>
     <row r="31">
@@ -20511,7 +20511,7 @@
         <v>5070.6</v>
       </c>
       <c r="GY31" t="n">
-        <v>3369.2</v>
+        <v>3367.3</v>
       </c>
     </row>
     <row r="32">
@@ -21757,7 +21757,7 @@
         <v>560.2</v>
       </c>
       <c r="GY33" t="n">
-        <v>618.8</v>
+        <v>623.3</v>
       </c>
     </row>
     <row r="34">
@@ -22380,7 +22380,7 @@
         <v>1413.9</v>
       </c>
       <c r="GY34" t="n">
-        <v>1463.5</v>
+        <v>1462.6</v>
       </c>
     </row>
     <row r="35">
@@ -23003,7 +23003,7 @@
         <v>85.5</v>
       </c>
       <c r="GY35" t="n">
-        <v>80.3666666666667</v>
+        <v>90.6</v>
       </c>
     </row>
     <row r="36">
@@ -24249,7 +24249,7 @@
         <v>850</v>
       </c>
       <c r="GY37" t="n">
-        <v>867.9</v>
+        <v>890.5</v>
       </c>
     </row>
     <row r="38">
@@ -24872,7 +24872,7 @@
         <v>3260.6</v>
       </c>
       <c r="GY38" t="n">
-        <v>3323.2</v>
+        <v>3342.9</v>
       </c>
     </row>
     <row r="39">
@@ -26996,7 +26996,7 @@
         <v>403.8</v>
       </c>
       <c r="GY42" t="n">
-        <v>683.7</v>
+        <v>683.6</v>
       </c>
     </row>
     <row r="43">
@@ -28242,7 +28242,7 @@
         <v>406.3</v>
       </c>
       <c r="GY44" t="n">
-        <v>692.3</v>
+        <v>692.2</v>
       </c>
     </row>
     <row r="45">
@@ -31559,7 +31559,7 @@
         <v>97.8</v>
       </c>
       <c r="GY59" t="n">
-        <v>105.1</v>
+        <v>104.5</v>
       </c>
     </row>
     <row r="60">
@@ -31780,7 +31780,7 @@
         <v>95.3</v>
       </c>
       <c r="GY60" t="n">
-        <v>82.4</v>
+        <v>82.1</v>
       </c>
     </row>
     <row r="61">
@@ -32001,7 +32001,7 @@
         <v>286.9</v>
       </c>
       <c r="GY61" t="n">
-        <v>238</v>
+        <v>237.2</v>
       </c>
     </row>
     <row r="62">
@@ -32222,7 +32222,7 @@
         <v>505</v>
       </c>
       <c r="GY62" t="n">
-        <v>431.3</v>
+        <v>429.7</v>
       </c>
     </row>
     <row r="63">
@@ -33908,7 +33908,7 @@
         <v>109.653</v>
       </c>
       <c r="GY66" t="n">
-        <v>124.27</v>
+        <v>124.335</v>
       </c>
     </row>
     <row r="67">
@@ -37646,7 +37646,7 @@
         <v>4976.66666666667</v>
       </c>
       <c r="GY72" t="n">
-        <v>5031.33333333333</v>
+        <v>5025.66666666667</v>
       </c>
     </row>
     <row r="73">
@@ -38269,7 +38269,7 @@
         <v>13671.3333333333</v>
       </c>
       <c r="GY73" t="n">
-        <v>13778.3333333333</v>
+        <v>13773.6666666667</v>
       </c>
     </row>
     <row r="74">
@@ -38892,7 +38892,7 @@
         <v>322875.333333333</v>
       </c>
       <c r="GY74" t="n">
-        <v>324766.555555556</v>
+        <v>317911</v>
       </c>
     </row>
     <row r="75">
@@ -39515,7 +39515,7 @@
         <v>0.0106010766854838</v>
       </c>
       <c r="GY75" t="n">
-        <v>0.0146167527152798</v>
+        <v>0.0148584946385095</v>
       </c>
     </row>
     <row r="76">
@@ -40138,7 +40138,7 @@
         <v>0.00947930812665287</v>
       </c>
       <c r="GY76" t="n">
-        <v>0.0156563913301293</v>
+        <v>0.0158068484542744</v>
       </c>
     </row>
     <row r="77">
@@ -40761,7 +40761,7 @@
         <v>0.00979116316539619</v>
       </c>
       <c r="GY77" t="n">
-        <v>0.00974006049182496</v>
+        <v>0.00986279752772545</v>
       </c>
     </row>
     <row r="78">
@@ -41384,7 +41384,7 @@
         <v>0.0153472039180007</v>
       </c>
       <c r="GY78" t="n">
-        <v>0.0172841160313526</v>
+        <v>0.0175269645608629</v>
       </c>
     </row>
     <row r="79">
@@ -42007,7 +42007,7 @@
         <v>0.0155281351781142</v>
       </c>
       <c r="GY79" t="n">
-        <v>0.016421172510237</v>
+        <v>0.0165635284167511</v>
       </c>
     </row>
     <row r="80">
@@ -42630,7 +42630,7 @@
         <v>0.0145277216114725</v>
       </c>
       <c r="GY80" t="n">
-        <v>0.0212199370268642</v>
+        <v>0.021931734440946</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Haver pull Q3 revision
</commit_message>
<xml_diff>
--- a/data/haver_pivoted.xlsx
+++ b/data/haver_pivoted.xlsx
@@ -2474,7 +2474,7 @@
         <v>22741</v>
       </c>
       <c r="GZ2" t="n">
-        <v>23173.5</v>
+        <v>23187</v>
       </c>
     </row>
     <row r="3">
@@ -3100,7 +3100,7 @@
         <v>19368.3</v>
       </c>
       <c r="GZ3" t="n">
-        <v>19465.2</v>
+        <v>19469.4</v>
       </c>
     </row>
     <row r="4">
@@ -3726,7 +3726,7 @@
         <v>117.546</v>
       </c>
       <c r="GZ4" t="n">
-        <v>119.19</v>
+        <v>119.237</v>
       </c>
     </row>
     <row r="5">
@@ -4352,7 +4352,7 @@
         <v>15681.7</v>
       </c>
       <c r="GZ5" t="n">
-        <v>15946.2</v>
+        <v>15952.4</v>
       </c>
     </row>
     <row r="6">
@@ -4978,7 +4978,7 @@
         <v>13665.6</v>
       </c>
       <c r="GZ6" t="n">
-        <v>13719.3</v>
+        <v>13723.7</v>
       </c>
     </row>
     <row r="7">
@@ -5604,7 +5604,7 @@
         <v>114.772</v>
       </c>
       <c r="GZ7" t="n">
-        <v>116.252</v>
+        <v>116.259</v>
       </c>
     </row>
     <row r="8">
@@ -6230,7 +6230,7 @@
         <v>115.228</v>
       </c>
       <c r="GZ8" t="n">
-        <v>116.539</v>
+        <v>116.58</v>
       </c>
     </row>
     <row r="9">
@@ -6856,7 +6856,7 @@
         <v>121.544</v>
       </c>
       <c r="GZ9" t="n">
-        <v>123.305</v>
+        <v>123.542</v>
       </c>
     </row>
     <row r="10">
@@ -7482,7 +7482,7 @@
         <v>121.425</v>
       </c>
       <c r="GZ10" t="n">
-        <v>122.996</v>
+        <v>123.296</v>
       </c>
     </row>
     <row r="11">
@@ -8108,7 +8108,7 @@
         <v>122.101</v>
       </c>
       <c r="GZ11" t="n">
-        <v>124.76</v>
+        <v>124.693</v>
       </c>
     </row>
     <row r="12">
@@ -9360,7 +9360,7 @@
         <v>730.5</v>
       </c>
       <c r="GZ13" t="n">
-        <v>740</v>
+        <v>786.3</v>
       </c>
     </row>
     <row r="14">
@@ -9986,7 +9986,7 @@
         <v>480.4</v>
       </c>
       <c r="GZ14" t="n">
-        <v>272.6</v>
+        <v>272.3</v>
       </c>
     </row>
     <row r="15">
@@ -10612,7 +10612,7 @@
         <v>4257.8</v>
       </c>
       <c r="GZ15" t="n">
-        <v>4038.8</v>
+        <v>4080.8</v>
       </c>
     </row>
     <row r="16">
@@ -11861,10 +11861,10 @@
         <v>2412.1</v>
       </c>
       <c r="GY17" t="n">
-        <v>2514.8</v>
+        <v>2532.5</v>
       </c>
       <c r="GZ17" t="n">
-        <v>2592.1</v>
+        <v>2619.2</v>
       </c>
     </row>
     <row r="18">
@@ -12490,7 +12490,7 @@
         <v>1636.3</v>
       </c>
       <c r="GZ18" t="n">
-        <v>1658.9</v>
+        <v>1661.6</v>
       </c>
     </row>
     <row r="19">
@@ -13116,7 +13116,7 @@
         <v>366.9</v>
       </c>
       <c r="GZ19" t="n">
-        <v>334.266666666667</v>
+        <v>384.5</v>
       </c>
     </row>
     <row r="20">
@@ -13742,7 +13742,7 @@
         <v>4015.9</v>
       </c>
       <c r="GZ20" t="n">
-        <v>4077</v>
+        <v>4083.7</v>
       </c>
     </row>
     <row r="21">
@@ -14365,10 +14365,10 @@
         <v>1539.2</v>
       </c>
       <c r="GY21" t="n">
-        <v>1564.2</v>
+        <v>1577.7</v>
       </c>
       <c r="GZ21" t="n">
-        <v>1594.5</v>
+        <v>1613.5</v>
       </c>
     </row>
     <row r="22">
@@ -14994,7 +14994,7 @@
         <v>114.753</v>
       </c>
       <c r="GZ22" t="n">
-        <v>116.232</v>
+        <v>116.239</v>
       </c>
     </row>
     <row r="23">
@@ -15620,7 +15620,7 @@
         <v>1563.3</v>
       </c>
       <c r="GZ23" t="n">
-        <v>1562.1</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="24">
@@ -16246,7 +16246,7 @@
         <v>2452.6</v>
       </c>
       <c r="GZ24" t="n">
-        <v>2514.9</v>
+        <v>2521.7</v>
       </c>
     </row>
     <row r="25">
@@ -16872,7 +16872,7 @@
         <v>1356.7</v>
       </c>
       <c r="GZ25" t="n">
-        <v>1340.4</v>
+        <v>1339.9</v>
       </c>
     </row>
     <row r="26">
@@ -17498,7 +17498,7 @@
         <v>2017.9</v>
       </c>
       <c r="GZ26" t="n">
-        <v>2039.6</v>
+        <v>2041.1</v>
       </c>
     </row>
     <row r="27">
@@ -18121,10 +18121,10 @@
         <v>1851.9</v>
       </c>
       <c r="GY27" t="n">
-        <v>1928.3</v>
+        <v>1946.1</v>
       </c>
       <c r="GZ27" t="n">
-        <v>1994.3</v>
+        <v>2019.3</v>
       </c>
     </row>
     <row r="28">
@@ -18750,7 +18750,7 @@
         <v>177.8</v>
       </c>
       <c r="GZ28" t="n">
-        <v>173.1</v>
+        <v>173</v>
       </c>
     </row>
     <row r="29">
@@ -19376,7 +19376,7 @@
         <v>275.1</v>
       </c>
       <c r="GZ29" t="n">
-        <v>248.866666666667</v>
+        <v>293.1</v>
       </c>
     </row>
     <row r="30">
@@ -19999,10 +19999,10 @@
         <v>1517.9</v>
       </c>
       <c r="GY30" t="n">
-        <v>1542.2</v>
+        <v>1555.7</v>
       </c>
       <c r="GZ30" t="n">
-        <v>1572.1</v>
+        <v>1591.1</v>
       </c>
     </row>
     <row r="31">
@@ -20628,7 +20628,7 @@
         <v>3372.3</v>
       </c>
       <c r="GZ31" t="n">
-        <v>3141.4</v>
+        <v>3136.6</v>
       </c>
     </row>
     <row r="32">
@@ -21880,7 +21880,7 @@
         <v>586.4</v>
       </c>
       <c r="GZ33" t="n">
-        <v>597.7</v>
+        <v>599.9</v>
       </c>
     </row>
     <row r="34">
@@ -22506,7 +22506,7 @@
         <v>1458.5</v>
       </c>
       <c r="GZ34" t="n">
-        <v>1485.8</v>
+        <v>1488.6</v>
       </c>
     </row>
     <row r="35">
@@ -23132,7 +23132,7 @@
         <v>91.9</v>
       </c>
       <c r="GZ35" t="n">
-        <v>85.4</v>
+        <v>91.4</v>
       </c>
     </row>
     <row r="36">
@@ -23758,7 +23758,7 @@
         <v>21.9</v>
       </c>
       <c r="GZ36" t="n">
-        <v>22.4</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="37">
@@ -24384,7 +24384,7 @@
         <v>885.5</v>
       </c>
       <c r="GZ37" t="n">
-        <v>897.4</v>
+        <v>944.3</v>
       </c>
     </row>
     <row r="38">
@@ -25010,7 +25010,7 @@
         <v>3337.6</v>
       </c>
       <c r="GZ38" t="n">
-        <v>3394.2</v>
+        <v>3448</v>
       </c>
     </row>
     <row r="39">
@@ -27146,7 +27146,7 @@
         <v>697</v>
       </c>
       <c r="GZ42" t="n">
-        <v>554.5</v>
+        <v>554.4</v>
       </c>
     </row>
     <row r="43">
@@ -28846,7 +28846,7 @@
         <v>14.1</v>
       </c>
       <c r="GZ46" t="n">
-        <v>15</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="47">
@@ -31760,7 +31760,7 @@
         <v>104.5</v>
       </c>
       <c r="GZ59" t="n">
-        <v>61.6</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="60">
@@ -31984,7 +31984,7 @@
         <v>82.1</v>
       </c>
       <c r="GZ60" t="n">
-        <v>50.1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61">
@@ -32432,7 +32432,7 @@
         <v>429.7</v>
       </c>
       <c r="GZ62" t="n">
-        <v>230.6</v>
+        <v>230.4</v>
       </c>
     </row>
     <row r="63">
@@ -32656,7 +32656,7 @@
         <v>5.8</v>
       </c>
       <c r="GZ63" t="n">
-        <v>5.8</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="64">
@@ -33504,7 +33504,7 @@
         <v>89.9</v>
       </c>
       <c r="GZ65" t="n">
-        <v>100.9</v>
+        <v>100.6</v>
       </c>
     </row>
     <row r="66">
@@ -34130,7 +34130,7 @@
         <v>128.939</v>
       </c>
       <c r="GZ66" t="n">
-        <v>140.094</v>
+        <v>135.881</v>
       </c>
     </row>
     <row r="67">
@@ -37886,7 +37886,7 @@
         <v>5023</v>
       </c>
       <c r="GZ72" t="n">
-        <v>5062.66666666667</v>
+        <v>5069</v>
       </c>
     </row>
     <row r="73">
@@ -38512,7 +38512,7 @@
         <v>13769.3333333333</v>
       </c>
       <c r="GZ73" t="n">
-        <v>14107</v>
+        <v>14088.3333333333</v>
       </c>
     </row>
     <row r="74">
@@ -39138,7 +39138,7 @@
         <v>318491.333333333</v>
       </c>
       <c r="GZ74" t="n">
-        <v>323230.555555556</v>
+        <v>321326.333333333</v>
       </c>
     </row>
     <row r="75">
@@ -39764,7 +39764,7 @@
         <v>0.0148498609983942</v>
       </c>
       <c r="GZ75" t="n">
-        <v>0.013986013986014</v>
+        <v>0.0143858574515507</v>
       </c>
     </row>
     <row r="76">
@@ -40390,7 +40390,7 @@
         <v>0.0157802971970722</v>
       </c>
       <c r="GZ76" t="n">
-        <v>0.012895131216673</v>
+        <v>0.0129561217021572</v>
       </c>
     </row>
     <row r="77">
@@ -41016,7 +41016,7 @@
         <v>0.010195940910884</v>
       </c>
       <c r="GZ77" t="n">
-        <v>0.0113774429826086</v>
+        <v>0.011733259277259</v>
       </c>
     </row>
     <row r="78">
@@ -41642,7 +41642,7 @@
         <v>0.0178200576137202</v>
       </c>
       <c r="GZ78" t="n">
-        <v>0.0144885802672283</v>
+        <v>0.016438491410518</v>
       </c>
     </row>
     <row r="79">
@@ -42268,7 +42268,7 @@
         <v>0.0167979969686567</v>
       </c>
       <c r="GZ79" t="n">
-        <v>0.0129380275890467</v>
+        <v>0.015408688490838</v>
       </c>
     </row>
     <row r="80">
@@ -42894,7 +42894,7 @@
         <v>0.0224844241977624</v>
       </c>
       <c r="GZ80" t="n">
-        <v>0.021777053422986</v>
+        <v>0.0212283273683262</v>
       </c>
     </row>
     <row r="81">
@@ -43517,10 +43517,10 @@
         <v>9888.1</v>
       </c>
       <c r="GY81" t="n">
-        <v>10087.8</v>
+        <v>10189.1</v>
       </c>
       <c r="GZ81" t="n">
-        <v>10327.7</v>
+        <v>10472.4</v>
       </c>
     </row>
     <row r="82">
@@ -44146,7 +44146,7 @@
         <v>1848.2</v>
       </c>
       <c r="GZ82" t="n">
-        <v>1850.6</v>
+        <v>1854.2</v>
       </c>
     </row>
     <row r="83">
@@ -44772,7 +44772,7 @@
         <v>716.3</v>
       </c>
       <c r="GZ83" t="n">
-        <v>729.3</v>
+        <v>728</v>
       </c>
     </row>
     <row r="84">
@@ -45398,7 +45398,7 @@
         <v>2932.1</v>
       </c>
       <c r="GZ84" t="n">
-        <v>2949.6</v>
+        <v>2949.8</v>
       </c>
     </row>
     <row r="85">
@@ -46024,7 +46024,7 @@
         <v>2359</v>
       </c>
       <c r="GZ85" t="n">
-        <v>2131.5</v>
+        <v>2440.4</v>
       </c>
     </row>
     <row r="86">

</xml_diff>